<commit_message>
fix gsbfrais and change diag_classe en cas_utilisation
</commit_message>
<xml_diff>
--- a/resssources/Tableau de synthese -Epreuve E4.xlsx
+++ b/resssources/Tableau de synthese -Epreuve E4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barck\Desktop\Portfolio\resssources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD820A4D-601C-4782-B386-9CB8013D9D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B108B6F5-86DB-466B-8A4B-9E4E787F8FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,12 +121,6 @@
 11/09/2024
 au
  18/09/2024</t>
-  </si>
-  <si>
-    <t>du 
-18/09/2024 
-au 
-02/09/2024</t>
   </si>
   <si>
     <t>du 
@@ -327,6 +321,12 @@
   </si>
   <si>
     <t>N° candidat : 02149903210</t>
+  </si>
+  <si>
+    <t>du 
+18/09/2024 
+au 
+02/10/2024</t>
   </si>
 </sst>
 </file>
@@ -926,27 +926,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -966,6 +949,23 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1186,8 +1186,8 @@
   </sheetPr>
   <dimension ref="A1:M992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1201,85 +1201,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="47" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="48"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A3" s="49" t="s">
-        <v>49</v>
+      <c r="A3" s="40" t="s">
+        <v>48</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="52" t="s">
-        <v>55</v>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43" t="s">
+        <v>54</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="53"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A4" s="42" t="s">
-        <v>51</v>
+      <c r="A4" s="32" t="s">
+        <v>50</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="43"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="23.25">
-      <c r="A5" s="44" t="s">
-        <v>50</v>
+      <c r="A5" s="35" t="s">
+        <v>49</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:13" ht="90" customHeight="1">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="47" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1302,8 +1302,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="324.75" customHeight="1">
-      <c r="A7" s="33"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1324,20 +1324,20 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
     </row>
     <row r="9" spans="1:13" ht="63.75" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>19</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="11" spans="1:13" ht="109.5" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>23</v>
@@ -1391,10 +1391,10 @@
     </row>
     <row r="12" spans="1:13" ht="125.25" customHeight="1">
       <c r="A12" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>20</v>
@@ -1413,10 +1413,10 @@
     </row>
     <row r="13" spans="1:13" ht="60">
       <c r="A13" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="14" spans="1:13" ht="30">
       <c r="A14" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="18">
         <v>45551</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="15" spans="1:13" ht="45">
       <c r="A15" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="18">
         <v>45565</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="16" spans="1:13" ht="106.5" customHeight="1">
       <c r="A16" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>20</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="17" spans="1:8" ht="98.25" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>20</v>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="18" spans="1:8" ht="64.5" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>20</v>
@@ -1527,10 +1527,10 @@
     </row>
     <row r="19" spans="1:8" ht="60">
       <c r="A19" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1543,10 +1543,10 @@
     </row>
     <row r="20" spans="1:8" ht="79.5" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>20</v>
@@ -1564,23 +1564,23 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="53"/>
+    </row>
+    <row r="22" spans="1:8" ht="90">
+      <c r="A22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="41"/>
-    </row>
-    <row r="22" spans="1:8" ht="90">
-      <c r="A22" s="15" t="s">
+      <c r="B22" s="28" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>38</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>20</v>
@@ -1599,10 +1599,10 @@
     </row>
     <row r="23" spans="1:8" ht="75">
       <c r="A23" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>20</v>
@@ -1616,23 +1616,23 @@
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="53"/>
+    </row>
+    <row r="25" spans="1:8" ht="81" customHeight="1">
+      <c r="A25" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="41"/>
-    </row>
-    <row r="25" spans="1:8" ht="81" customHeight="1">
-      <c r="A25" s="15" t="s">
+      <c r="B25" s="28" t="s">
         <v>41</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>42</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>20</v>
@@ -1651,10 +1651,10 @@
     </row>
     <row r="26" spans="1:8" ht="60">
       <c r="A26" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>20</v>
@@ -11329,6 +11329,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A1:F1"/>
@@ -11336,11 +11341,6 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A24:H24"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>